<commit_message>
Atualizado por script em 04-01-2024 20:45
</commit_message>
<xml_diff>
--- a/2023/israel_ligat-ha-al_2023-2024.xlsx
+++ b/2023/israel_ligat-ha-al_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V97"/>
+  <dimension ref="A1:V98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -757,22 +757,22 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>H. Beer Sheva</t>
+          <t>Netanya</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Hapoel Hadera</t>
+          <t>Maccabi Bnei Raina</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>1.41</v>
+        <v>2.09</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -780,15 +780,15 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>1.34</v>
+        <v>1.73</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>23/08/2023 14:56</t>
+          <t>26/08/2023 15:32</t>
         </is>
       </c>
       <c r="N4" t="n">
-        <v>4.54</v>
+        <v>3.3</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -796,15 +796,15 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>5.09</v>
+        <v>3.7</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>24/08/2023 19:03</t>
+          <t>26/08/2023 15:32</t>
         </is>
       </c>
       <c r="R4" t="n">
-        <v>7.49</v>
+        <v>3.66</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -812,16 +812,16 @@
         </is>
       </c>
       <c r="T4" t="n">
-        <v>8.470000000000001</v>
+        <v>5.01</v>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>23/08/2023 14:56</t>
+          <t>26/08/2023 17:28</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/h-beer-sheva-hapoel-hadera/Qkt5hlII/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/netanya-maccabi-bnei-raina/CtFNAVXn/</t>
         </is>
       </c>
     </row>
@@ -849,22 +849,22 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Netanya</t>
+          <t>H. Beer Sheva</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Maccabi Bnei Raina</t>
+          <t>Hapoel Hadera</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>2.09</v>
+        <v>1.41</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -872,15 +872,15 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>1.73</v>
+        <v>1.34</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>26/08/2023 15:32</t>
+          <t>23/08/2023 14:56</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>3.3</v>
+        <v>4.54</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -888,15 +888,15 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>3.7</v>
+        <v>5.09</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>26/08/2023 15:32</t>
+          <t>24/08/2023 19:03</t>
         </is>
       </c>
       <c r="R5" t="n">
-        <v>3.66</v>
+        <v>7.49</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
@@ -904,16 +904,16 @@
         </is>
       </c>
       <c r="T5" t="n">
-        <v>5.01</v>
+        <v>8.470000000000001</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>26/08/2023 17:28</t>
+          <t>23/08/2023 14:56</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/netanya-maccabi-bnei-raina/CtFNAVXn/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/h-beer-sheva-hapoel-hadera/Qkt5hlII/</t>
         </is>
       </c>
     </row>
@@ -3241,22 +3241,22 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>SC Ashdod</t>
+          <t>Hapoel Haifa</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Hapoel Hadera</t>
+          <t>Maccabi Bnei Raina</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J31" t="n">
-        <v>2.13</v>
+        <v>2.07</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -3264,15 +3264,15 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.81</v>
+        <v>2.11</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>30/09/2023 18:41</t>
+          <t>30/09/2023 18:44</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>3.34</v>
+        <v>3.37</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3280,7 +3280,7 @@
         </is>
       </c>
       <c r="P31" t="n">
-        <v>3.58</v>
+        <v>3.32</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
@@ -3288,7 +3288,7 @@
         </is>
       </c>
       <c r="R31" t="n">
-        <v>3.48</v>
+        <v>3.63</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
@@ -3296,7 +3296,7 @@
         </is>
       </c>
       <c r="T31" t="n">
-        <v>4.6</v>
+        <v>3.72</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
@@ -3305,7 +3305,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/sc-ashdod-hapoel-hadera/jXkLL732/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-haifa-maccabi-bnei-raina/xU1wcOQ1/</t>
         </is>
       </c>
     </row>
@@ -3333,22 +3333,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Hapoel Haifa</t>
+          <t>SC Ashdod</t>
         </is>
       </c>
       <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Hapoel Hadera</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
         <v>1</v>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Maccabi Bnei Raina</t>
-        </is>
-      </c>
-      <c r="I32" t="n">
-        <v>2</v>
-      </c>
       <c r="J32" t="n">
-        <v>2.07</v>
+        <v>2.13</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
@@ -3356,48 +3356,48 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>2.11</v>
+        <v>1.81</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
+          <t>30/09/2023 18:41</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>23/09/2023 18:13</t>
+        </is>
+      </c>
+      <c r="P32" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
           <t>30/09/2023 18:44</t>
         </is>
       </c>
-      <c r="N32" t="n">
-        <v>3.37</v>
-      </c>
-      <c r="O32" t="inlineStr">
+      <c r="R32" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="S32" t="inlineStr">
         <is>
           <t>23/09/2023 18:13</t>
         </is>
       </c>
-      <c r="P32" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="Q32" t="inlineStr">
+      <c r="T32" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="U32" t="inlineStr">
         <is>
           <t>30/09/2023 18:44</t>
         </is>
       </c>
-      <c r="R32" t="n">
-        <v>3.63</v>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>23/09/2023 18:13</t>
-        </is>
-      </c>
-      <c r="T32" t="n">
-        <v>3.72</v>
-      </c>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>30/09/2023 18:44</t>
-        </is>
-      </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-haifa-maccabi-bnei-raina/xU1wcOQ1/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/sc-ashdod-hapoel-hadera/jXkLL732/</t>
         </is>
       </c>
     </row>
@@ -4437,71 +4437,71 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Maccabi Petah Tikva</t>
+          <t>Hapoel Hadera</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Netanya</t>
+          <t>Maccabi Bnei Raina</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J44" t="n">
-        <v>2.42</v>
+        <v>2.99</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>04/12/2023 12:06</t>
+          <t>02/12/2023 18:13</t>
         </is>
       </c>
       <c r="L44" t="n">
-        <v>2.82</v>
+        <v>2.63</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>05/12/2023 17:52</t>
+          <t>05/12/2023 17:57</t>
         </is>
       </c>
       <c r="N44" t="n">
-        <v>3.21</v>
+        <v>3.14</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>04/12/2023 12:06</t>
+          <t>02/12/2023 18:13</t>
         </is>
       </c>
       <c r="P44" t="n">
-        <v>3.35</v>
+        <v>3.18</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>05/12/2023 17:51</t>
+          <t>05/12/2023 17:50</t>
         </is>
       </c>
       <c r="R44" t="n">
-        <v>2.89</v>
+        <v>2.39</v>
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>04/12/2023 12:06</t>
+          <t>02/12/2023 18:13</t>
         </is>
       </c>
       <c r="T44" t="n">
-        <v>2.56</v>
+        <v>2.86</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>05/12/2023 17:52</t>
+          <t>05/12/2023 17:50</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/maccabi-petah-tikva-netanya/Acl9Ase1/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-hadera-maccabi-bnei-raina/txPwQMfl/</t>
         </is>
       </c>
     </row>
@@ -4529,71 +4529,71 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Hapoel Hadera</t>
+          <t>Maccabi Petah Tikva</t>
         </is>
       </c>
       <c r="G45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Netanya</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
         <v>0</v>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Maccabi Bnei Raina</t>
-        </is>
-      </c>
-      <c r="I45" t="n">
-        <v>2</v>
-      </c>
       <c r="J45" t="n">
-        <v>2.99</v>
+        <v>2.42</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>02/12/2023 18:13</t>
+          <t>04/12/2023 12:06</t>
         </is>
       </c>
       <c r="L45" t="n">
-        <v>2.63</v>
+        <v>2.82</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>05/12/2023 17:57</t>
+          <t>05/12/2023 17:52</t>
         </is>
       </c>
       <c r="N45" t="n">
-        <v>3.14</v>
+        <v>3.21</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>02/12/2023 18:13</t>
+          <t>04/12/2023 12:06</t>
         </is>
       </c>
       <c r="P45" t="n">
-        <v>3.18</v>
+        <v>3.35</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>05/12/2023 17:50</t>
+          <t>05/12/2023 17:51</t>
         </is>
       </c>
       <c r="R45" t="n">
-        <v>2.39</v>
+        <v>2.89</v>
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>02/12/2023 18:13</t>
+          <t>04/12/2023 12:06</t>
         </is>
       </c>
       <c r="T45" t="n">
-        <v>2.86</v>
+        <v>2.56</v>
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>05/12/2023 17:50</t>
+          <t>05/12/2023 17:52</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-hadera-maccabi-bnei-raina/txPwQMfl/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/maccabi-petah-tikva-netanya/Acl9Ase1/</t>
         </is>
       </c>
     </row>
@@ -5725,71 +5725,71 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>SC Ashdod</t>
+          <t>Hapoel Hadera</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Hapoel Jerusalem</t>
+          <t>Hapoel Petah Tikva</t>
         </is>
       </c>
       <c r="I58" t="n">
         <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>2.63</v>
+        <v>2.33</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>12/12/2023 05:12</t>
+          <t>15/12/2023 14:42</t>
         </is>
       </c>
       <c r="L58" t="n">
-        <v>2.5</v>
+        <v>2.42</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>16/12/2023 16:59</t>
+          <t>16/12/2023 16:55</t>
         </is>
       </c>
       <c r="N58" t="n">
-        <v>3.06</v>
+        <v>3.35</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>12/12/2023 05:12</t>
+          <t>15/12/2023 14:42</t>
         </is>
       </c>
       <c r="P58" t="n">
-        <v>2.92</v>
+        <v>3.31</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>16/12/2023 16:59</t>
+          <t>16/12/2023 16:55</t>
         </is>
       </c>
       <c r="R58" t="n">
-        <v>2.73</v>
+        <v>2.91</v>
       </c>
       <c r="S58" t="inlineStr">
         <is>
-          <t>12/12/2023 05:12</t>
+          <t>15/12/2023 14:42</t>
         </is>
       </c>
       <c r="T58" t="n">
-        <v>3.32</v>
+        <v>3.03</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>16/12/2023 16:59</t>
+          <t>16/12/2023 16:55</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/sc-ashdod-hapoel-jerusalem/4vxUzv96/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-hadera-hapoel-petah-tikva/b1yYZcOC/</t>
         </is>
       </c>
     </row>
@@ -5909,71 +5909,71 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Hapoel Hadera</t>
+          <t>SC Ashdod</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Hapoel Petah Tikva</t>
+          <t>Hapoel Jerusalem</t>
         </is>
       </c>
       <c r="I60" t="n">
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>2.33</v>
+        <v>2.63</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>15/12/2023 14:42</t>
+          <t>12/12/2023 05:12</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>2.42</v>
+        <v>2.5</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>16/12/2023 16:55</t>
+          <t>16/12/2023 16:59</t>
         </is>
       </c>
       <c r="N60" t="n">
-        <v>3.35</v>
+        <v>3.06</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>15/12/2023 14:42</t>
+          <t>12/12/2023 05:12</t>
         </is>
       </c>
       <c r="P60" t="n">
-        <v>3.31</v>
+        <v>2.92</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>16/12/2023 16:55</t>
+          <t>16/12/2023 16:59</t>
         </is>
       </c>
       <c r="R60" t="n">
-        <v>2.91</v>
+        <v>2.73</v>
       </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>15/12/2023 14:42</t>
+          <t>12/12/2023 05:12</t>
         </is>
       </c>
       <c r="T60" t="n">
-        <v>3.03</v>
+        <v>3.32</v>
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>16/12/2023 16:55</t>
+          <t>16/12/2023 16:59</t>
         </is>
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-hadera-hapoel-petah-tikva/b1yYZcOC/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/sc-ashdod-hapoel-jerusalem/4vxUzv96/</t>
         </is>
       </c>
     </row>
@@ -7013,22 +7013,22 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Hapoel Haifa</t>
+          <t>SC Ashdod</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Netanya</t>
+          <t>Sakhnin</t>
         </is>
       </c>
       <c r="I72" t="n">
         <v>1</v>
       </c>
       <c r="J72" t="n">
-        <v>2.74</v>
+        <v>2.1</v>
       </c>
       <c r="K72" t="inlineStr">
         <is>
@@ -7036,15 +7036,15 @@
         </is>
       </c>
       <c r="L72" t="n">
-        <v>3.04</v>
+        <v>2.19</v>
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>23/12/2023 16:58</t>
+          <t>23/12/2023 16:55</t>
         </is>
       </c>
       <c r="N72" t="n">
-        <v>3.18</v>
+        <v>3.22</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -7052,15 +7052,15 @@
         </is>
       </c>
       <c r="P72" t="n">
-        <v>3.37</v>
+        <v>3.32</v>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>23/12/2023 16:56</t>
+          <t>23/12/2023 16:55</t>
         </is>
       </c>
       <c r="R72" t="n">
-        <v>2.53</v>
+        <v>3.48</v>
       </c>
       <c r="S72" t="inlineStr">
         <is>
@@ -7068,16 +7068,16 @@
         </is>
       </c>
       <c r="T72" t="n">
-        <v>2.39</v>
+        <v>3.5</v>
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>23/12/2023 16:58</t>
+          <t>23/12/2023 16:55</t>
         </is>
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-haifa-netanya/fsfyV8xo/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/sc-ashdod-sakhnin/8prJghFo/</t>
         </is>
       </c>
     </row>
@@ -7105,22 +7105,22 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>SC Ashdod</t>
+          <t>Hapoel Haifa</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Sakhnin</t>
+          <t>Netanya</t>
         </is>
       </c>
       <c r="I73" t="n">
         <v>1</v>
       </c>
       <c r="J73" t="n">
-        <v>2.1</v>
+        <v>2.74</v>
       </c>
       <c r="K73" t="inlineStr">
         <is>
@@ -7128,15 +7128,15 @@
         </is>
       </c>
       <c r="L73" t="n">
-        <v>2.19</v>
+        <v>3.04</v>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>23/12/2023 16:55</t>
+          <t>23/12/2023 16:58</t>
         </is>
       </c>
       <c r="N73" t="n">
-        <v>3.22</v>
+        <v>3.18</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -7144,15 +7144,15 @@
         </is>
       </c>
       <c r="P73" t="n">
-        <v>3.32</v>
+        <v>3.37</v>
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>23/12/2023 16:55</t>
+          <t>23/12/2023 16:56</t>
         </is>
       </c>
       <c r="R73" t="n">
-        <v>3.48</v>
+        <v>2.53</v>
       </c>
       <c r="S73" t="inlineStr">
         <is>
@@ -7160,16 +7160,16 @@
         </is>
       </c>
       <c r="T73" t="n">
-        <v>3.5</v>
+        <v>2.39</v>
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>23/12/2023 16:55</t>
+          <t>23/12/2023 16:58</t>
         </is>
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/sc-ashdod-sakhnin/8prJghFo/</t>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-haifa-netanya/fsfyV8xo/</t>
         </is>
       </c>
     </row>
@@ -9378,6 +9378,98 @@
       <c r="V97" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-petah-tikva-maccabi-haifa/IqTde5jj/</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>israel</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>ligat-ha-al</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>45295.8125</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Hapoel Haifa</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>3</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Beitar Jerusalem</t>
+        </is>
+      </c>
+      <c r="I98" t="n">
+        <v>2</v>
+      </c>
+      <c r="J98" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>31/12/2024 19:17</t>
+        </is>
+      </c>
+      <c r="L98" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>04/01/2024 19:26</t>
+        </is>
+      </c>
+      <c r="N98" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>31/12/2024 19:17</t>
+        </is>
+      </c>
+      <c r="P98" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>04/01/2024 19:26</t>
+        </is>
+      </c>
+      <c r="R98" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>31/12/2024 19:17</t>
+        </is>
+      </c>
+      <c r="T98" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="U98" t="inlineStr">
+        <is>
+          <t>04/01/2024 19:26</t>
+        </is>
+      </c>
+      <c r="V98" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/israel/ligat-ha-al/hapoel-haifa-beitar-jerusalem/OtKnISc3/</t>
         </is>
       </c>
     </row>

</xml_diff>